<commit_message>
started to add postgres data:
</commit_message>
<xml_diff>
--- a/data_df.xlsx
+++ b/data_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\Calorie-Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AB1B58-A3BA-4263-916B-0A4E0AEFBB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33FB5D1-BBDB-47CC-9E05-0527FB273208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calorie_df" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Snacks_Red</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -908,29 +911,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -970,8 +976,14 @@
       <c r="M1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44697</v>
       </c>
@@ -1011,8 +1023,14 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>162.4</v>
+      </c>
+      <c r="O2">
+        <v>12863</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44698</v>
       </c>
@@ -1052,8 +1070,14 @@
       <c r="M3">
         <v>700</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>161.80000000000001</v>
+      </c>
+      <c r="O3">
+        <v>13593</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44699</v>
       </c>
@@ -1093,8 +1117,14 @@
       <c r="M4">
         <v>658</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>161.4</v>
+      </c>
+      <c r="O4">
+        <v>12128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44700</v>
       </c>
@@ -1133,6 +1163,12 @@
       </c>
       <c r="M5">
         <v>190</v>
+      </c>
+      <c r="N5">
+        <v>161</v>
+      </c>
+      <c r="O5">
+        <v>11987</v>
       </c>
     </row>
   </sheetData>
@@ -1144,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,6 +1303,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1275,7 +1312,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,5 +1411,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>